<commit_message>
Added model report for color classification
</commit_message>
<xml_diff>
--- a/model_report_color_prediction.xlsx
+++ b/model_report_color_prediction.xlsx
@@ -662,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -694,10 +694,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -709,150 +705,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
@@ -893,6 +745,150 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,7 +1172,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,21 +1188,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1233,12 +1229,12 @@
       <c r="I2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="68" t="s">
+      <c r="J2" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -1256,21 +1252,21 @@
       <c r="F3" s="10">
         <v>16</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="11">
         <v>0.96454472199838837</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="11">
         <v>0.96419272098789532</v>
       </c>
       <c r="I3" s="6">
         <v>0.95899999999999996</v>
       </c>
-      <c r="J3" s="68">
+      <c r="J3" s="18">
         <v>0.95799999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1294,11 +1290,11 @@
       <c r="H4" s="3">
         <v>0.94482165712789112</v>
       </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1322,11 +1318,11 @@
       <c r="H5" s="3">
         <v>0.94549275768257768</v>
       </c>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1350,11 +1346,11 @@
       <c r="H6" s="3">
         <v>0.93820638504461251</v>
       </c>
-      <c r="I6" s="71"/>
-      <c r="J6" s="72"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1378,11 +1374,11 @@
       <c r="H7" s="3">
         <v>0.95638532773650664</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="72"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1406,11 +1402,11 @@
       <c r="H8" s="3">
         <v>0.96023925148785461</v>
       </c>
-      <c r="I8" s="71"/>
-      <c r="J8" s="72"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1434,11 +1430,11 @@
       <c r="H9" s="3">
         <v>0.94884046950725676</v>
       </c>
-      <c r="I9" s="71"/>
-      <c r="J9" s="72"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1462,11 +1458,11 @@
       <c r="H10" s="3">
         <v>0.96040619676280936</v>
       </c>
-      <c r="I10" s="71"/>
-      <c r="J10" s="72"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1490,11 +1486,11 @@
       <c r="H11" s="3">
         <v>0.95318234939560265</v>
       </c>
-      <c r="I11" s="71"/>
-      <c r="J11" s="72"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1518,11 +1514,11 @@
       <c r="H12" s="3">
         <v>0.93877832010487616</v>
       </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="72"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1546,11 +1542,11 @@
       <c r="H13" s="3">
         <v>0.95863030196871746</v>
       </c>
-      <c r="I13" s="71"/>
-      <c r="J13" s="72"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1574,11 +1570,11 @@
       <c r="H14" s="3">
         <v>0.9578927733203072</v>
       </c>
-      <c r="I14" s="71"/>
-      <c r="J14" s="72"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1602,11 +1598,11 @@
       <c r="H15" s="3">
         <v>0.93928880670435577</v>
       </c>
-      <c r="I15" s="71"/>
-      <c r="J15" s="72"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1630,11 +1626,11 @@
       <c r="H16" s="3">
         <v>0.94159504307212971</v>
       </c>
-      <c r="I16" s="71"/>
-      <c r="J16" s="72"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1658,11 +1654,11 @@
       <c r="H17" s="3">
         <v>0.93824667434404874</v>
       </c>
-      <c r="I17" s="71"/>
-      <c r="J17" s="72"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1686,11 +1682,11 @@
       <c r="H18" s="3">
         <v>0.94386539854273832</v>
       </c>
-      <c r="I18" s="71"/>
-      <c r="J18" s="72"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1714,11 +1710,11 @@
       <c r="H19" s="5">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I19" s="71"/>
-      <c r="J19" s="72"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1742,11 +1738,11 @@
       <c r="H20" s="5">
         <v>0.95</v>
       </c>
-      <c r="I20" s="71"/>
-      <c r="J20" s="72"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1770,11 +1766,11 @@
       <c r="H21" s="5">
         <v>0.95</v>
       </c>
-      <c r="I21" s="71"/>
-      <c r="J21" s="72"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1798,11 +1794,11 @@
       <c r="H22" s="5">
         <v>0.91</v>
       </c>
-      <c r="I22" s="71"/>
-      <c r="J22" s="72"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1826,327 +1822,301 @@
       <c r="H23" s="8">
         <v>0.9587</v>
       </c>
-      <c r="I23" s="71"/>
-      <c r="J23" s="72"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="72"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="22"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30" t="s">
+      <c r="B25" s="71"/>
+      <c r="C25" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="34" t="s">
+      <c r="D25" s="72"/>
+      <c r="E25" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="72"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="31" t="s">
+      <c r="B26" s="74"/>
+      <c r="C26" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="26" t="s">
+      <c r="D26" s="56"/>
+      <c r="E26" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="72"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="20" t="s">
+      <c r="D27" s="66"/>
+      <c r="E27" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="20" t="s">
+      <c r="F27" s="65"/>
+      <c r="G27" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="21"/>
+      <c r="H27" s="65"/>
       <c r="I27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J27" s="68" t="s">
+      <c r="J27" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="75" t="s">
+      <c r="A28" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="14">
         <v>3</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="22">
+      <c r="D28" s="67"/>
+      <c r="E28" s="78">
         <v>0.99099999999999999</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="11">
+      <c r="F28" s="79"/>
+      <c r="G28" s="78">
         <v>0.99099999999999999</v>
       </c>
-      <c r="H28" s="12"/>
+      <c r="H28" s="79"/>
       <c r="I28" s="6">
         <v>0.98499999999999999</v>
       </c>
-      <c r="J28" s="68">
+      <c r="J28" s="18">
         <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="72"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="22"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41" t="s">
+      <c r="B30" s="54"/>
+      <c r="C30" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41" t="s">
+      <c r="D30" s="54"/>
+      <c r="E30" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="72"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31" t="s">
+      <c r="B31" s="56"/>
+      <c r="C31" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31" t="s">
+      <c r="D31" s="56"/>
+      <c r="E31" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="71"/>
-      <c r="J31" s="72"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="22"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="76" t="s">
+      <c r="A32" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="45" t="s">
+      <c r="C32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="56" t="s">
+      <c r="D32" s="39"/>
+      <c r="E32" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="57"/>
-      <c r="G32" s="56" t="s">
+      <c r="F32" s="38"/>
+      <c r="G32" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="57"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="72"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="22"/>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="27" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="9">
         <v>10</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="58">
+      <c r="D33" s="41"/>
+      <c r="E33" s="34">
         <v>0.96199999999999997</v>
       </c>
-      <c r="F33" s="59"/>
-      <c r="G33" s="58">
+      <c r="F33" s="33"/>
+      <c r="G33" s="34">
         <v>0.96199999999999997</v>
       </c>
-      <c r="H33" s="59"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="72"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="72"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="22"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="52"/>
-      <c r="C35" s="53" t="s">
+      <c r="B35" s="46"/>
+      <c r="C35" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="52"/>
-      <c r="E35" s="53" t="s">
+      <c r="D35" s="46"/>
+      <c r="E35" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="72"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="60" t="s">
+      <c r="A36" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="58" t="s">
+      <c r="B36" s="33"/>
+      <c r="C36" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="59"/>
-      <c r="E36" s="58" t="s">
+      <c r="D36" s="33"/>
+      <c r="E36" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="71"/>
-      <c r="J36" s="72"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="22"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="76" t="s">
+      <c r="A37" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="57"/>
-      <c r="E37" s="56" t="s">
+      <c r="D37" s="38"/>
+      <c r="E37" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="57"/>
-      <c r="G37" s="56" t="s">
+      <c r="F37" s="38"/>
+      <c r="G37" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="H37" s="57"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="72"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="22"/>
     </row>
     <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="78" t="s">
+      <c r="A38" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="79">
+      <c r="B38" s="29">
         <v>0.5</v>
       </c>
-      <c r="C38" s="58">
+      <c r="C38" s="34">
         <v>1000</v>
       </c>
-      <c r="D38" s="59"/>
-      <c r="E38" s="58">
+      <c r="D38" s="33"/>
+      <c r="E38" s="34">
         <v>0.89400000000000002</v>
       </c>
-      <c r="F38" s="59"/>
-      <c r="G38" s="58">
+      <c r="F38" s="33"/>
+      <c r="G38" s="34">
         <v>0.89300000000000002</v>
       </c>
-      <c r="H38" s="59"/>
-      <c r="I38" s="80"/>
-      <c r="J38" s="81"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="E31:H31"/>
+  <mergeCells count="40">
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E27:F27"/>
@@ -2160,6 +2130,33 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="E25:H25"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
providing CNN option for color recognition
</commit_message>
<xml_diff>
--- a/model_report_color_prediction.xlsx
+++ b/model_report_color_prediction.xlsx
@@ -155,9 +155,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,8 +189,22 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +229,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="35">
     <border>
@@ -659,10 +679,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -670,31 +691,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -745,6 +754,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -764,6 +793,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -847,6 +882,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -883,15 +924,58 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1171,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,21 +1272,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1226,47 +1310,47 @@
       <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <v>3</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="7">
         <v>32</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="7">
         <v>16</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="28">
         <v>0.96454472199838837</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="86">
         <v>0.96419272098789532</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="29">
         <v>0.95899999999999996</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="90">
         <v>0.95799999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1284,17 +1368,17 @@
       <c r="F4" s="2">
         <v>16</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="30">
         <v>0.9452054794520548</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="87">
         <v>0.94482165712789112</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1312,17 +1396,17 @@
       <c r="F5" s="2">
         <v>16</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="30">
         <v>0.9460112812248187</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="87">
         <v>0.94549275768257768</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1340,17 +1424,17 @@
       <c r="F6" s="2">
         <v>16</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="30">
         <v>0.93875906526994357</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="87">
         <v>0.93820638504461251</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1368,17 +1452,17 @@
       <c r="F7" s="2">
         <v>16</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="30">
         <v>0.95648670427074944</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="87">
         <v>0.95638532773650664</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1396,17 +1480,17 @@
       <c r="F8" s="2">
         <v>16</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="30">
         <v>0.96051571313456885</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="87">
         <v>0.96023925148785461</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="22"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1424,17 +1508,17 @@
       <c r="F9" s="2">
         <v>16</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="30">
         <v>0.94923448831587431</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="87">
         <v>0.94884046950725676</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1452,17 +1536,17 @@
       <c r="F10" s="2">
         <v>16</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="30">
         <v>0.96051571313456885</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="87">
         <v>0.96040619676280936</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="22"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1480,17 +1564,17 @@
       <c r="F11" s="2">
         <v>16</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="30">
         <v>0.95326349717969383</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="87">
         <v>0.95318234939560265</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="22"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1508,17 +1592,17 @@
       <c r="F12" s="2">
         <v>16</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="30">
         <v>0.93956486704270747</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="87">
         <v>0.93877832010487616</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="22"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1536,17 +1620,17 @@
       <c r="F13" s="2">
         <v>16</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="30">
         <v>0.95890410958904104</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="87">
         <v>0.95863030196871746</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="22"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1564,17 +1648,17 @@
       <c r="F14" s="2">
         <v>16</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="30">
         <v>0.95809830781627725</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="87">
         <v>0.9578927733203072</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="22"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1592,17 +1676,17 @@
       <c r="F15" s="2">
         <v>16</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="30">
         <v>0.93956486704270747</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="87">
         <v>0.93928880670435577</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="22"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1620,17 +1704,17 @@
       <c r="F16" s="2">
         <v>16</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="30">
         <v>0.94198227236099918</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="87">
         <v>0.94159504307212971</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="32"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1648,17 +1732,17 @@
       <c r="F17" s="2">
         <v>16</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="30">
         <v>0.93875906526994357</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="87">
         <v>0.93824667434404874</v>
       </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="22"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1676,444 +1760,448 @@
       <c r="F18" s="2">
         <v>16</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="30">
         <v>0.94439967767929089</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="87">
         <v>0.94386539854273832</v>
       </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="22"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="A19" s="96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="97">
         <v>3</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="97">
         <v>32</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="97">
         <v>20</v>
       </c>
-      <c r="G19" s="5">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="22"/>
+      <c r="G19" s="98">
+        <v>0.97340000000000004</v>
+      </c>
+      <c r="H19" s="99">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="I19" s="100">
+        <v>0.96109999999999995</v>
+      </c>
+      <c r="J19" s="101">
+        <v>0.96</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>3</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="2">
         <v>32</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>20</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="33">
         <v>0.95</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="88">
         <v>0.95</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>3</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="2">
         <v>32</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>20</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="33">
         <v>0.95</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="88">
         <v>0.95</v>
       </c>
-      <c r="I21" s="21"/>
-      <c r="J21" s="22"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="32"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>3</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="2">
         <v>32</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>20</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="33">
         <v>0.91200000000000003</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="88">
         <v>0.91</v>
       </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="7" t="s">
+      <c r="A23" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>3</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <v>32</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="5">
         <v>30</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="34">
         <v>0.95899999999999996</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="89">
         <v>0.9587</v>
       </c>
-      <c r="I23" s="21"/>
-      <c r="J23" s="22"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="32"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="59" t="s">
+      <c r="A24" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="22"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="72" t="s">
+      <c r="B25" s="79"/>
+      <c r="C25" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="72"/>
-      <c r="E25" s="75" t="s">
+      <c r="D25" s="80"/>
+      <c r="E25" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="76"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="22"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="18"/>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="56" t="s">
+      <c r="B26" s="82"/>
+      <c r="C26" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="56"/>
-      <c r="E26" s="68" t="s">
+      <c r="D26" s="62"/>
+      <c r="E26" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="22"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="18"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="64" t="s">
+      <c r="D27" s="74"/>
+      <c r="E27" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="65"/>
-      <c r="G27" s="64" t="s">
+      <c r="F27" s="71"/>
+      <c r="G27" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="65"/>
-      <c r="I27" s="6" t="s">
+      <c r="H27" s="71"/>
+      <c r="I27" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J27" s="18" t="s">
+      <c r="J27" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="10">
         <v>3</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="67"/>
-      <c r="E28" s="78">
+      <c r="D28" s="75"/>
+      <c r="E28" s="72">
         <v>0.99099999999999999</v>
       </c>
-      <c r="F28" s="79"/>
-      <c r="G28" s="78">
+      <c r="F28" s="73"/>
+      <c r="G28" s="92">
         <v>0.99099999999999999</v>
       </c>
-      <c r="H28" s="79"/>
-      <c r="I28" s="6">
+      <c r="H28" s="93"/>
+      <c r="I28" s="35">
         <v>0.98499999999999999</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="91">
         <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="22"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="18"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54" t="s">
+      <c r="B30" s="60"/>
+      <c r="C30" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54" t="s">
+      <c r="D30" s="60"/>
+      <c r="E30" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="22"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="18"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56" t="s">
+      <c r="B31" s="62"/>
+      <c r="C31" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56" t="s">
+      <c r="D31" s="62"/>
+      <c r="E31" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="22"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="18"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="37" t="s">
+      <c r="D32" s="45"/>
+      <c r="E32" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="38"/>
-      <c r="G32" s="37" t="s">
+      <c r="F32" s="42"/>
+      <c r="G32" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="38"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="22"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="18"/>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="6">
         <v>10</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="34">
+      <c r="D33" s="47"/>
+      <c r="E33" s="43">
         <v>0.96199999999999997</v>
       </c>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34">
+      <c r="F33" s="44"/>
+      <c r="G33" s="94">
         <v>0.96199999999999997</v>
       </c>
-      <c r="H33" s="33"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="22"/>
+      <c r="H33" s="95"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="22"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="18"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="46"/>
-      <c r="C35" s="47" t="s">
+      <c r="B35" s="52"/>
+      <c r="C35" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="46"/>
-      <c r="E35" s="47" t="s">
+      <c r="D35" s="52"/>
+      <c r="E35" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="22"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="18"/>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="C36" s="34" t="s">
+      <c r="B36" s="37"/>
+      <c r="C36" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="34" t="s">
+      <c r="D36" s="37"/>
+      <c r="E36" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="22"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="18"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="37" t="s">
+      <c r="D37" s="42"/>
+      <c r="E37" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="38"/>
-      <c r="G37" s="37" t="s">
+      <c r="F37" s="42"/>
+      <c r="G37" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="H37" s="38"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="22"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="18"/>
     </row>
     <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="29">
+      <c r="B38" s="25">
         <v>0.5</v>
       </c>
-      <c r="C38" s="34">
+      <c r="C38" s="38">
         <v>1000</v>
       </c>
-      <c r="D38" s="33"/>
-      <c r="E38" s="34">
+      <c r="D38" s="37"/>
+      <c r="E38" s="43">
         <v>0.89400000000000002</v>
       </c>
-      <c r="F38" s="33"/>
-      <c r="G38" s="34">
+      <c r="F38" s="44"/>
+      <c r="G38" s="94">
         <v>0.89300000000000002</v>
       </c>
-      <c r="H38" s="33"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="31"/>
+      <c r="H38" s="95"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="40">

</xml_diff>